<commit_message>
+ 3.1 support for BPV, EDA, EMG, Settings ignored for now
</commit_message>
<xml_diff>
--- a/inst/extdata/MW/3.1_EDA.xlsx
+++ b/inst/extdata/MW/3.1_EDA.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gepelman\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GH\psyphr_dev\psyphr.read\inst\extdata\MW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{185A04CD-6AFA-4E4B-B216-07A7DAB62CE5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DC41F6-C5B3-458F-8BFF-8249300E7DA6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{D4616601-C271-47A1-9F63-FBA97D425D5B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D4616601-C271-47A1-9F63-FBA97D425D5B}"/>
   </bookViews>
   <sheets>
     <sheet name="EDA Stats" sheetId="1" r:id="rId1"/>
     <sheet name="SCR Stats" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -611,14 +610,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4810122-4FF3-4741-AEEC-E107C7B4CE83}">
   <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="9" width="13.5703125" customWidth="1"/>
+    <col min="1" max="9" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -632,7 +631,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -646,7 +645,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -660,7 +659,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -674,7 +673,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -688,7 +687,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -702,7 +701,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -716,7 +715,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -730,7 +729,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -744,7 +743,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -758,7 +757,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -772,7 +771,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -786,7 +785,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
@@ -800,7 +799,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -814,7 +813,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -828,7 +827,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -842,7 +841,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -856,7 +855,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
@@ -870,7 +869,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -884,7 +883,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
@@ -898,7 +897,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -912,7 +911,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
@@ -926,7 +925,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -936,7 +935,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>35</v>
       </c>
@@ -950,7 +949,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
@@ -964,7 +963,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -974,7 +973,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>38</v>
       </c>
@@ -988,7 +987,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>39</v>
       </c>
@@ -1002,7 +1001,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>40</v>
       </c>
@@ -1016,7 +1015,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
@@ -1030,7 +1029,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>43</v>
       </c>
@@ -1044,7 +1043,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -1058,7 +1057,7 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>45</v>
       </c>
@@ -1072,7 +1071,7 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
@@ -1086,7 +1085,7 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>47</v>
       </c>
@@ -1100,7 +1099,7 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
@@ -1114,7 +1113,7 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>50</v>
       </c>
@@ -1128,7 +1127,7 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>52</v>
       </c>
@@ -1142,7 +1141,7 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>54</v>
       </c>
@@ -1156,7 +1155,7 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1166,7 +1165,7 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>55</v>
       </c>
@@ -1195,7 +1194,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>56</v>
       </c>
@@ -1208,7 +1207,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>57</v>
       </c>
@@ -1221,7 +1220,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>22</v>
       </c>
@@ -1250,7 +1249,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>58</v>
       </c>
@@ -1263,7 +1262,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>59</v>
       </c>
@@ -1276,7 +1275,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>24</v>
       </c>
@@ -1305,7 +1304,7 @@
         <v>436.67200000000003</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>60</v>
       </c>
@@ -1334,7 +1333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>61</v>
       </c>
@@ -1363,7 +1362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>62</v>
       </c>
@@ -1392,7 +1391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>63</v>
       </c>
@@ -1421,7 +1420,7 @@
         <v>7.6368739999999997</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>64</v>
       </c>
@@ -1450,7 +1449,7 @@
         <v>7.7419890000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>65</v>
       </c>
@@ -1479,7 +1478,7 @@
         <v>9.1617069999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1489,7 +1488,7 @@
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1499,7 +1498,7 @@
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1509,7 +1508,7 @@
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1519,7 +1518,7 @@
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1529,7 +1528,7 @@
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1539,7 +1538,7 @@
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1549,7 +1548,7 @@
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1559,7 +1558,7 @@
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1569,7 +1568,7 @@
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1579,7 +1578,7 @@
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1589,7 +1588,7 @@
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1599,7 +1598,7 @@
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1609,7 +1608,7 @@
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1619,7 +1618,7 @@
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1629,7 +1628,7 @@
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1639,7 +1638,7 @@
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1649,7 +1648,7 @@
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1659,7 +1658,7 @@
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1669,7 +1668,7 @@
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1679,7 +1678,7 @@
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1689,7 +1688,7 @@
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1699,7 +1698,7 @@
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1709,7 +1708,7 @@
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1719,7 +1718,7 @@
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1729,7 +1728,7 @@
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1739,7 +1738,7 @@
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1749,7 +1748,7 @@
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -1759,7 +1758,7 @@
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1769,7 +1768,7 @@
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -1779,7 +1778,7 @@
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -1789,7 +1788,7 @@
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -1799,7 +1798,7 @@
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -1809,7 +1808,7 @@
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -1819,7 +1818,7 @@
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -1829,7 +1828,7 @@
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -1839,7 +1838,7 @@
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -1849,7 +1848,7 @@
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -1859,7 +1858,7 @@
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -1869,7 +1868,7 @@
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -1879,7 +1878,7 @@
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -1889,7 +1888,7 @@
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -1899,7 +1898,7 @@
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -1909,7 +1908,7 @@
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -1919,7 +1918,7 @@
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -1929,7 +1928,7 @@
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -1939,7 +1938,7 @@
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -1949,7 +1948,7 @@
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -1959,7 +1958,7 @@
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -1969,7 +1968,7 @@
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -1979,7 +1978,7 @@
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -1989,7 +1988,7 @@
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -1999,7 +1998,7 @@
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2018,14 +2017,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EBFE7FA-91BC-4748-B14D-EDF18D3BA25E}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="10" width="13.5703125" customWidth="1"/>
+    <col min="1" max="10" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2057,7 +2056,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2089,7 +2088,7 @@
         <v>0.45900000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2121,7 +2120,7 @@
         <v>0.52100000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -2153,7 +2152,7 @@
         <v>0.39100000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -2185,7 +2184,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -2217,7 +2216,7 @@
         <v>0.41599999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -2249,7 +2248,7 @@
         <v>0.26800000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -2281,7 +2280,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -2313,7 +2312,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -2345,7 +2344,7 @@
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -2377,7 +2376,7 @@
         <v>0.10100000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>4</v>
       </c>
@@ -2409,7 +2408,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -2441,7 +2440,7 @@
         <v>5.7000000000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>4</v>
       </c>
@@ -2473,7 +2472,7 @@
         <v>0.17799999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>4</v>
       </c>
@@ -2505,7 +2504,7 @@
         <v>0.32800000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -2537,7 +2536,7 @@
         <v>0.14199999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>4</v>
       </c>
@@ -2569,7 +2568,7 @@
         <v>0.17499999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>5</v>
       </c>
@@ -2601,7 +2600,7 @@
         <v>0.17199999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>5</v>
       </c>
@@ -2633,7 +2632,7 @@
         <v>1.1220000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>5</v>
       </c>
@@ -2665,7 +2664,7 @@
         <v>0.17599999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>5</v>
       </c>
@@ -2697,7 +2696,7 @@
         <v>0.157</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>6</v>
       </c>
@@ -2729,7 +2728,7 @@
         <v>0.155</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>6</v>
       </c>
@@ -2761,7 +2760,7 @@
         <v>0.249</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>7</v>
       </c>
@@ -2793,7 +2792,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>7</v>
       </c>
@@ -2825,7 +2824,7 @@
         <v>0.73299999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>8</v>
       </c>
@@ -2857,7 +2856,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>8</v>
       </c>
@@ -2889,7 +2888,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>8</v>
       </c>
@@ -2924,16 +2923,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E103EDD-314C-4C78-B82D-0E651A6E7B66}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>